<commit_message>
cleans formatting on data dictionaries and makes few edits to methods
</commit_message>
<xml_diff>
--- a/metadata/project-metadata.xlsx
+++ b/metadata/project-metadata.xlsx
@@ -1,28 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/zoe_kanavas_water_ca_gov/Documents/Documents/Water Data Consortium Projects/urban-water-drought-data/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/urban-water-drought-data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F035E0-F781-1641-B04C-AE2836CF1309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8365A556-F683-8640-B678-E2F434B6DE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="15720" tabRatio="834" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="31900" windowHeight="21260" tabRatio="834" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dataset" sheetId="13" r:id="rId1"/>
-    <sheet name="personnel" sheetId="1" r:id="rId2"/>
-    <sheet name="title" sheetId="2" r:id="rId3"/>
-    <sheet name="keyword_set" sheetId="3" r:id="rId4"/>
-    <sheet name="license" sheetId="4" r:id="rId5"/>
-    <sheet name="project" sheetId="11" r:id="rId6"/>
-    <sheet name="funding" sheetId="5" r:id="rId7"/>
-    <sheet name="maintenance" sheetId="6" r:id="rId8"/>
-    <sheet name="coverage" sheetId="7" r:id="rId9"/>
-    <sheet name="taxonomic_coverage" sheetId="8" r:id="rId10"/>
+    <sheet name="personnel" sheetId="1" r:id="rId1"/>
+    <sheet name="title" sheetId="2" r:id="rId2"/>
+    <sheet name="keyword_set" sheetId="3" r:id="rId3"/>
+    <sheet name="license" sheetId="4" r:id="rId4"/>
+    <sheet name="funding" sheetId="5" r:id="rId5"/>
+    <sheet name="maintenance" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>first_name</t>
   </si>
@@ -51,9 +47,6 @@
     <t>orcid</t>
   </si>
   <si>
-    <t>organization</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -63,9 +56,6 @@
     <t>keyword</t>
   </si>
   <si>
-    <t>keywordThesaurus</t>
-  </si>
-  <si>
     <t xml:space="preserve">default_license </t>
   </si>
   <si>
@@ -102,74 +92,56 @@
     <t>update_frequency</t>
   </si>
   <si>
-    <t>geographic_description</t>
-  </si>
-  <si>
-    <t>west_bounding_coordinate</t>
-  </si>
-  <si>
-    <t>east_bounding_coordinate</t>
-  </si>
-  <si>
-    <t>north_bounding_coordinate</t>
-  </si>
-  <si>
-    <t>south_bounding_coordinate</t>
-  </si>
-  <si>
-    <t>begin_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>common_name</t>
-  </si>
-  <si>
-    <t>kingdom</t>
-  </si>
-  <si>
-    <t>phylum</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genus </t>
-  </si>
-  <si>
-    <t xml:space="preserve">species </t>
-  </si>
-  <si>
-    <t>taxon_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">organization </t>
   </si>
   <si>
-    <t>CVPIA_common_species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">type </t>
-  </si>
-  <si>
-    <t xml:space="preserve">geometry </t>
+    <t xml:space="preserve">ongoing </t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>CCBY</t>
+  </si>
+  <si>
+    <t>insert data steward contact</t>
+  </si>
+  <si>
+    <t>Making Urban Water Data Public and Useful for Understanding Drought Impacts</t>
+  </si>
+  <si>
+    <t>Urban Water Data for Drought</t>
+  </si>
+  <si>
+    <t>urban water management plan</t>
+  </si>
+  <si>
+    <t>annual water supply and demand assessment</t>
+  </si>
+  <si>
+    <t>water use efficiency</t>
+  </si>
+  <si>
+    <t>electronic annual report</t>
+  </si>
+  <si>
+    <t>state standard shortage level</t>
+  </si>
+  <si>
+    <t>demand reduction</t>
+  </si>
+  <si>
+    <t>supply augmentation</t>
+  </si>
+  <si>
+    <t>facility</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -192,32 +164,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -233,28 +186,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -637,146 +579,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC88997-D746-4692-9A7F-1A0E218D4835}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{1233EF59-08AA-402F-97DC-7F1A6FD6CFFE}">
-      <formula1>" Point, LineString, LinearRing, Polygon, Multipoint, MultiLineString, MultiPolygon, MultiGeometry"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{0D49A741-B9FC-40CC-92FB-9400626C24F0}">
-      <formula1>"tabular, vector, raster"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
-    <col min="2" max="2" width="20.375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="21" style="9" customWidth="1"/>
-    <col min="4" max="8" width="10.5" style="9"/>
-    <col min="9" max="9" width="10.375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="32.625" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{1B42BD17-108B-4DE3-B195-41BB977BD94A}">
-      <formula1>"chinook, steelhead, delta_smelt, white_sturgeon, green_sturgeon"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="27.375" customWidth="1"/>
-    <col min="6" max="6" width="27" style="7" customWidth="1"/>
+    <col min="1" max="2" width="10.5" style="2"/>
+    <col min="3" max="3" width="18.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="2"/>
+    <col min="5" max="5" width="27.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -790,30 +639,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="34.875" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+    </row>
+    <row r="2" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -821,67 +675,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.625" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="9"/>
-    <col min="4" max="4" width="15.125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26" style="9" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="2"/>
+    <col min="4" max="4" width="15.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>14</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -895,94 +791,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CC0791-3488-4AA1-946D-D16C61358F1D}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9" style="9"/>
-    <col min="3" max="3" width="9" style="7"/>
-    <col min="4" max="4" width="9" style="9"/>
-    <col min="5" max="5" width="14.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{8F71D943-5F40-45B5-8A1F-11A7EFDD12D7}">
-      <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="7"/>
+    <col min="1" max="1" width="13" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -995,25 +843,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="2"/>
+    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1032,79 +890,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="53.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="6"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4:G8 G3" xr:uid="{D0FABE90-94BB-4510-8A04-3DED000903A4}">
-      <formula1>F2</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>